<commit_message>
updated BoM and added bluetooth files
</commit_message>
<xml_diff>
--- a/BoM.xlsx
+++ b/BoM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/asood08_student_ubc_ca/Documents/Documents/Adarsh/Uni Courses/Third Year/Sem 2/ELEC 391/c5-elec391/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{681B96A5-E031-497D-B0F4-A01718FBABDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="8_{681B96A5-E031-497D-B0F4-A01718FBABDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F5B9C99-F6AE-4124-9B93-5621F37935F4}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13920" xr2:uid="{57B1A439-6759-4F50-B30A-DEEC5208487C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>SI No</t>
   </si>
@@ -53,15 +53,6 @@
     <t>Magnetic Encoders</t>
   </si>
   <si>
-    <t>Logic Level Shifter (TXB0104PWR)</t>
-  </si>
-  <si>
-    <t>Limit Switch</t>
-  </si>
-  <si>
-    <t>Ultrasonic Sensor</t>
-  </si>
-  <si>
     <t>Cost/Piece</t>
   </si>
   <si>
@@ -72,13 +63,28 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>LM7805</t>
+  </si>
+  <si>
+    <t>SlipRing</t>
+  </si>
+  <si>
+    <t>Ultrasonic Sensor (HC-SR04)</t>
+  </si>
+  <si>
+    <t>Logic Level Shifter (TXB0104PWR + BOB)</t>
+  </si>
+  <si>
+    <t>IR sensor for Homing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,8 +92,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -112,6 +124,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -125,11 +143,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -145,6 +164,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -464,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECE199EF-59F8-4C09-B6FB-442FEDE88BC1}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -487,16 +510,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
@@ -504,7 +527,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -513,7 +536,6 @@
         <v>5</v>
       </c>
       <c r="E2" s="1">
-        <f>13</f>
         <v>13</v>
       </c>
       <c r="F2" s="1">
@@ -538,29 +560,29 @@
         <v>13</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F6" si="0">C3/D3*E3</f>
+        <f t="shared" ref="F3:F8" si="0">C3/D3*E3</f>
         <v>6.5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A4" s="2">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="4">
         <v>2</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="4">
         <v>2</v>
       </c>
-      <c r="E4" s="1">
-        <v>14</v>
-      </c>
-      <c r="F4" s="1">
-        <f>C4/D4*E4</f>
-        <v>14</v>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <f>C4/D4*E4*0</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
@@ -568,20 +590,20 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
       </c>
       <c r="D5" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="0"/>
-        <v>1.6666666666666665</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
@@ -589,7 +611,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -598,24 +620,66 @@
         <v>1</v>
       </c>
       <c r="E6" s="1">
-        <v>1.49</v>
+        <v>5.32</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>1.49</v>
+        <v>5.32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A7" s="2">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2.82</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>2.82</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="D8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="3">
-        <f>SUM(E2:E6)</f>
-        <v>51.49</v>
-      </c>
-      <c r="F8" s="3">
-        <f>SUM(F2:F6)</f>
-        <v>26.256666666666668</v>
+      <c r="A8" s="2">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>15</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="3">
+        <f>SUM(E2:E8)</f>
+        <v>62.14</v>
+      </c>
+      <c r="F11" s="3">
+        <f>SUM(F2:F8)</f>
+        <v>34.840000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>